<commit_message>
Check code for errors when running
</commit_message>
<xml_diff>
--- a/compras/templates/compras/mail/compras.xlsx
+++ b/compras/templates/compras/mail/compras.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,93 +426,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B1" t="inlineStr">
+        <is>
+          <t>pan</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>44819</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Huevos</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>44819</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Arroz</t>
         </is>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>44663</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Pollo</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>44663</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>25</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Verduras</t>
-        </is>
-      </c>
       <c r="C3" s="1" t="n">
-        <v>44663</v>
+        <v>44819</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Flores para la mesa</t>
+          <t>Mantequilla</t>
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44663</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>27</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Pitayas</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>44663</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>29</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Lentejas</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>44664</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>30</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Zanahoria</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>44669</v>
+        <v>44819</v>
       </c>
     </row>
   </sheetData>

</xml_diff>